<commit_message>
Minor docs added more test cases to spreadsheet
</commit_message>
<xml_diff>
--- a/example/Sample_Bar_template_v2023_1.xlsx
+++ b/example/Sample_Bar_template_v2023_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brist\Documents\GitHub\rsoxs_scans\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nistgov-my.sharepoint.com/personal/bbp_nist_gov/Documents/BP_NISTSoftware/BPWINPC01_Git/rsoxs_scans/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E36585-B06A-48A1-B455-5D04BF8C010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{90E36585-B06A-48A1-B455-5D04BF8C010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9013265A-467F-4066-80F8-AFEDE03D53F0}"/>
   <bookViews>
-    <workbookView xWindow="36110" yWindow="-5130" windowWidth="30950" windowHeight="16050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="240">
   <si>
     <t>Do not change the format of the Acquisitions or Samples tab.Other tabs can be added and edited as needed.</t>
   </si>
@@ -796,6 +796,15 @@
   <si>
     <t>Information about possible acquisitions and arguments are given in this template and on the wiki</t>
   </si>
+  <si>
+    <t>WAXSNEXAFS</t>
+  </si>
+  <si>
+    <t>WAXS_liquid</t>
+  </si>
+  <si>
+    <t>SAXS_liquid</t>
+  </si>
 </sst>
 </file>
 
@@ -865,7 +874,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -984,12 +993,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -999,26 +1002,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -1030,13 +1025,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1436,7 +1424,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -38731,16 +38719,16 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C8:C572">
-    <cfRule type="duplicateValues" dxfId="11" priority="5" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="5" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D193">
-    <cfRule type="duplicateValues" dxfId="10" priority="4" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="4" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C7">
-    <cfRule type="duplicateValues" dxfId="9" priority="2" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D7">
-    <cfRule type="duplicateValues" dxfId="8" priority="1" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
   <dataValidations count="16">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O573:O1662 M233:N1662 C8:E1662 C6:E7" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -38816,8 +38804,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:V688"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -38846,75 +38834,75 @@
     <col min="22" max="22" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="37" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:22" s="35" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="34" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="17" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" s="17" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>98</v>
       </c>
@@ -40730,13 +40718,64 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B67" s="3"/>
+      <c r="A67" s="26">
+        <v>62</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67">
+        <v>62</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B68" s="3"/>
+      <c r="A68" s="26">
+        <v>63</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E68">
+        <v>63</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B69" s="3"/>
+      <c r="A69" s="26">
+        <v>64</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E69">
+        <v>64</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B70" s="3"/>
@@ -42597,27 +42636,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:N1 J6:N1048576">
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
       <formula>"rsoxs"=$D1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:M1 Q1 H1:I1 H6:I1048576 Q6:Q1048576 L6:M1048576">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>"nexafs"=$D1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1 G1:K1 P1 P6:P1048576 G6:K1048576 N6:N1048576">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
       <formula>"spiral"=$D1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1 F6:F1048576">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>OR($D1="rsoxs", $D1="nexafs")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E1004">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT(ISBLANK($B6))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42682,25 +42721,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="15"/>
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:18" ht="30.75" x14ac:dyDescent="0.4">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="15"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -44069,7 +44108,7 @@
       </c>
       <c r="G49" s="16"/>
     </row>
-    <row r="50" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
Add tests for #7 group selection
</commit_message>
<xml_diff>
--- a/example/Sample_Bar_template_v2023_1.xlsx
+++ b/example/Sample_Bar_template_v2023_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nistgov-my.sharepoint.com/personal/bbp_nist_gov/Documents/BP_NISTSoftware/BPWINPC01_Git/rsoxs_scans/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{90E36585-B06A-48A1-B455-5D04BF8C010C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9013265A-467F-4066-80F8-AFEDE03D53F0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BE9207-22EC-44D7-9AD3-89C1FC3090A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="241">
   <si>
     <t>Do not change the format of the Acquisitions or Samples tab.Other tabs can be added and edited as needed.</t>
   </si>
@@ -805,6 +805,9 @@
   <si>
     <t>SAXS_liquid</t>
   </si>
+  <si>
+    <t>groupA</t>
+  </si>
 </sst>
 </file>
 
@@ -1013,7 +1016,35 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -38719,16 +38750,16 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C8:C572">
-    <cfRule type="duplicateValues" dxfId="8" priority="5" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="5" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D193">
-    <cfRule type="duplicateValues" dxfId="7" priority="4" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="4" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C7">
-    <cfRule type="duplicateValues" dxfId="6" priority="2" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="2" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D7">
-    <cfRule type="duplicateValues" dxfId="5" priority="1" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
   <dataValidations count="16">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O573:O1662 M233:N1662 C8:E1662 C6:E7" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -38804,8 +38835,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:V688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -39263,7 +39294,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>53</v>
@@ -39284,7 +39315,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>54</v>
@@ -39306,7 +39337,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>53</v>
@@ -39333,7 +39364,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>54</v>
@@ -39354,7 +39385,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>53</v>
@@ -39375,7 +39406,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>54</v>
@@ -39402,7 +39433,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>53</v>
@@ -39426,7 +39457,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="26">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>54</v>
@@ -39453,7 +39484,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="26">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>53</v>
@@ -39480,7 +39511,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="26">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>54</v>
@@ -39501,7 +39532,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="26">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>53</v>
@@ -39528,7 +39559,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="26">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>54</v>
@@ -39555,7 +39586,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="26">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>53</v>
@@ -39582,7 +39613,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="26">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>54</v>
@@ -39609,7 +39640,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="26">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>53</v>
@@ -39636,7 +39667,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="26">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>54</v>
@@ -39660,7 +39691,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="26">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>53</v>
@@ -39689,7 +39720,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="26">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>54</v>
@@ -39716,7 +39747,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="26">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>53</v>
@@ -39737,7 +39768,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="26">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>54</v>
@@ -39761,7 +39792,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="26">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>53</v>
@@ -39785,7 +39816,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="26">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>54</v>
@@ -39809,7 +39840,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="26">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>53</v>
@@ -39833,7 +39864,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="26">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>54</v>
@@ -39857,7 +39888,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>53</v>
@@ -39881,7 +39912,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>54</v>
@@ -39905,7 +39936,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="26">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>53</v>
@@ -39929,7 +39960,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="26">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>54</v>
@@ -39950,7 +39981,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="26">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>53</v>
@@ -39971,7 +40002,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="26">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>54</v>
@@ -39992,7 +40023,7 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="26">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>53</v>
@@ -40016,7 +40047,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="26">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>54</v>
@@ -40040,7 +40071,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="26">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>53</v>
@@ -40064,7 +40095,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="26">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>54</v>
@@ -40091,7 +40122,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="26">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>53</v>
@@ -40118,7 +40149,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="26">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>54</v>
@@ -40145,7 +40176,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="26">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>53</v>
@@ -40172,7 +40203,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="26">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>54</v>
@@ -40199,7 +40230,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="26">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>53</v>
@@ -40226,7 +40257,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="26">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>54</v>
@@ -40256,7 +40287,7 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="26">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>53</v>
@@ -40280,7 +40311,7 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="26">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>54</v>
@@ -40306,7 +40337,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="26">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>53</v>
@@ -40329,7 +40360,7 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="26">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>54</v>
@@ -40349,7 +40380,7 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="26">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>53</v>
@@ -40372,7 +40403,7 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="26">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>54</v>
@@ -40395,7 +40426,7 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="26">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>53</v>
@@ -40418,7 +40449,7 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="26">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>54</v>
@@ -40441,7 +40472,7 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="26">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>53</v>
@@ -40464,7 +40495,7 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" s="26">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>54</v>
@@ -40487,7 +40518,7 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="26">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>53</v>
@@ -40510,7 +40541,7 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="26">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>54</v>
@@ -40530,7 +40561,7 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" s="26">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>53</v>
@@ -40553,7 +40584,7 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="26">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>54</v>
@@ -40576,7 +40607,7 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="26">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>53</v>
@@ -40599,7 +40630,7 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="26">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>54</v>
@@ -40619,7 +40650,7 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="26">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>53</v>
@@ -40639,7 +40670,7 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" s="26">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>54</v>
@@ -40659,7 +40690,7 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" s="26">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>53</v>
@@ -40677,9 +40708,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="26">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>54</v>
@@ -40697,9 +40728,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="26">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>53</v>
@@ -40717,9 +40748,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="26">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>54</v>
@@ -40737,9 +40768,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="26">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68" s="10" t="s">
         <v>54</v>
@@ -40757,9 +40788,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="26">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B69" s="10" t="s">
         <v>54</v>
@@ -40777,37 +40808,132 @@
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A70" s="26">
+        <v>64</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D70" t="s">
+        <v>62</v>
+      </c>
+      <c r="E70">
+        <v>65</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G70" t="s">
+        <v>81</v>
+      </c>
+      <c r="T70" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A71" s="26">
+        <v>65</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C71" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" t="s">
+        <v>62</v>
+      </c>
+      <c r="E71">
+        <v>66</v>
+      </c>
+      <c r="F71" t="s">
+        <v>80</v>
+      </c>
+      <c r="G71" t="s">
+        <v>81</v>
+      </c>
+      <c r="T71" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A72" s="26">
+        <v>66</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C72" t="s">
+        <v>61</v>
+      </c>
+      <c r="D72" t="s">
+        <v>62</v>
+      </c>
+      <c r="E72">
+        <v>67</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G72" t="s">
+        <v>82</v>
+      </c>
+      <c r="T72" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A73" s="26">
+        <v>67</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C73" t="s">
+        <v>60</v>
+      </c>
+      <c r="D73" t="s">
+        <v>62</v>
+      </c>
+      <c r="E73">
+        <v>68</v>
+      </c>
+      <c r="F73" t="s">
+        <v>80</v>
+      </c>
+      <c r="G73" t="s">
+        <v>81</v>
+      </c>
+      <c r="H73">
+        <v>5</v>
+      </c>
+      <c r="T73" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B76" s="3"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B77" s="3"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B78" s="3"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B79" s="3"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B80" s="3"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2">
@@ -42636,28 +42762,48 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:N1 J6:N1048576">
-    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
       <formula>"rsoxs"=$D1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:M1 Q1 H1:I1 H6:I1048576 Q6:Q1048576 L6:M1048576">
-    <cfRule type="expression" dxfId="3" priority="6">
+  <conditionalFormatting sqref="L1:M1 Q1 H1:I1 H6:I69 Q6:Q1048576 L6:M1048576 H74:I1048576">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>"nexafs"=$D1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1 G1:K1 P1 P6:P1048576 G6:K1048576 N6:N1048576">
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="N1 G1:K1 P1 P6:P1048576 G6:K69 N6:N1048576 G74:K1048576 J70:K73">
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
       <formula>"spiral"=$D1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1 F6:F1048576">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="F1 F6:F69 F74:F1048576">
+    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
       <formula>OR($D1="rsoxs", $D1="nexafs")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:E1004">
+  <conditionalFormatting sqref="C6:E69 C74:E1004">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>NOT(ISBLANK($B6))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H70:I73">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>"nexafs"=$D70</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G70:I73">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>"spiral"=$D70</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F70:F73">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>OR($D70="rsoxs", $D70="nexafs")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C70:E73">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>NOT(ISBLANK($B6))</formula>
+      <formula>NOT(ISBLANK($B70))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
removing invalid rows of sample spreadsheet
</commit_message>
<xml_diff>
--- a/example/Sample_Bar_template_v2023_1.xlsx
+++ b/example/Sample_Bar_template_v2023_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brist\Documents\GitHub\rsoxs_scans\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEA8132-9062-4C85-8E24-F13261828D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDF4215-BB9E-472E-ABEA-AF21DC0FDB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36110" yWindow="-5130" windowWidth="30950" windowHeight="16050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="242">
   <si>
     <t>Do not change the format of the Acquisitions or Samples tab.Other tabs can be added and edited as needed.</t>
   </si>
@@ -809,28 +809,7 @@
     <t>groupA</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>diodeRangeTest</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>invalidParamTest</t>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>rat</t>
-  </si>
-  <si>
-    <t>mat</t>
   </si>
 </sst>
 </file>
@@ -1037,49 +1016,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -38813,16 +38750,16 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C8:C572">
-    <cfRule type="duplicateValues" dxfId="18" priority="5" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="5" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D193">
-    <cfRule type="duplicateValues" dxfId="17" priority="4" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="4" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C7">
-    <cfRule type="duplicateValues" dxfId="16" priority="2" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="2" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D7">
-    <cfRule type="duplicateValues" dxfId="15" priority="1" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
   <dataValidations count="16">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O573:O1662 M233:N1662 C8:E1662 C6:E7" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -38893,10 +38830,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116CCDDD-7003-4820-AA86-27B44350A195}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:V688"/>
+  <dimension ref="A1:V685"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R77" sqref="R76:R77"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -39946,7 +39883,7 @@
         <v>77</v>
       </c>
       <c r="T29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
@@ -39973,7 +39910,7 @@
         <v>78</v>
       </c>
       <c r="T30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
@@ -40000,7 +39937,7 @@
         <v>77</v>
       </c>
       <c r="T31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
@@ -40027,7 +39964,7 @@
         <v>79</v>
       </c>
       <c r="T32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
@@ -40988,103 +40925,13 @@
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A74" s="25">
-        <v>68</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C74" t="s">
-        <v>61</v>
-      </c>
-      <c r="D74" t="s">
-        <v>63</v>
-      </c>
-      <c r="E74">
-        <v>27</v>
-      </c>
-      <c r="F74" t="s">
-        <v>65</v>
-      </c>
-      <c r="H74" t="s">
-        <v>243</v>
-      </c>
-      <c r="I74" t="s">
-        <v>241</v>
-      </c>
-      <c r="M74">
-        <v>3111</v>
-      </c>
-      <c r="T74" t="s">
-        <v>244</v>
-      </c>
+      <c r="B74" s="3"/>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A75" s="25">
-        <v>69</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C75" t="s">
-        <v>61</v>
-      </c>
-      <c r="D75" t="s">
-        <v>63</v>
-      </c>
-      <c r="E75">
-        <v>27</v>
-      </c>
-      <c r="F75" t="s">
-        <v>65</v>
-      </c>
-      <c r="G75" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="L75">
-        <v>223</v>
-      </c>
-      <c r="M75">
-        <v>11</v>
-      </c>
-      <c r="T75" t="s">
-        <v>244</v>
-      </c>
+      <c r="B75" s="3"/>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A76" s="25">
-        <v>70</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C76" t="s">
-        <v>60</v>
-      </c>
-      <c r="D76" t="s">
-        <v>62</v>
-      </c>
-      <c r="E76">
-        <v>68</v>
-      </c>
-      <c r="F76" t="s">
-        <v>80</v>
-      </c>
-      <c r="G76" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="H76" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="I76" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="O76">
-        <v>-600</v>
-      </c>
-      <c r="T76" t="s">
-        <v>244</v>
-      </c>
+      <c r="B76" s="3"/>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B77" s="3"/>
@@ -42913,89 +42760,50 @@
     <row r="685" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B685" s="3"/>
     </row>
-    <row r="686" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B686" s="3"/>
-    </row>
-    <row r="687" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B687" s="3"/>
-    </row>
-    <row r="688" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B688" s="3"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="J1:N1 J6:N1048576">
-    <cfRule type="expression" dxfId="14" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="18" stopIfTrue="1">
       <formula>"rsoxs"=$D1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:M1 Q1 H1:I1 H6:I69 Q6:Q1048576 L6:M1048576 H74:I1048576">
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="7" priority="16">
       <formula>"nexafs"=$D1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1 G1:K1 P1 P6:P1048576 G6:K69 N6:N1048576 G74:K1048576 J70:K73">
-    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
+  <conditionalFormatting sqref="N1 G1:K1 P1 G6:K69 J70:K73 P6:P1048576 N6:N1048576 G74:K1048576">
+    <cfRule type="expression" dxfId="6" priority="15" stopIfTrue="1">
       <formula>"spiral"=$D1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1 F6:F69 F77:F1048576">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+  <conditionalFormatting sqref="F1 F6:F69 F74:F1048576">
+    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
       <formula>OR($D1="rsoxs", $D1="nexafs")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:E69 C77:E1004">
-    <cfRule type="expression" dxfId="10" priority="11">
+  <conditionalFormatting sqref="C6:E69 C74:E1001">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>NOT(ISBLANK($B6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70:I73">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>"nexafs"=$D70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70:I73">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="9" stopIfTrue="1">
       <formula>"spiral"=$D70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70:F73">
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="8" stopIfTrue="1">
       <formula>OR($D70="rsoxs", $D70="nexafs")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:E73">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="0" priority="7">
       <formula>NOT(ISBLANK($B70))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F74">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
-      <formula>OR($D74="rsoxs", $D74="nexafs")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C74:E74">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>NOT(ISBLANK($B74))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F75">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
-      <formula>OR($D75="rsoxs", $D75="nexafs")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C75:E75">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>NOT(ISBLANK($B75))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F76">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>OR($D76="rsoxs", $D76="nexafs")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C76:E76">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>NOT(ISBLANK($B76))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -43012,13 +42820,13 @@
           <x14:formula1>
             <xm:f>Bar!$C$4:$C$250</xm:f>
           </x14:formula1>
-          <xm:sqref>B656:B896</xm:sqref>
+          <xm:sqref>B653:B893</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AC3EBA0B-0DD4-40E5-BE31-66F1E5977B51}">
           <x14:formula1>
             <xm:f>Bar!$C$4:$C$450</xm:f>
           </x14:formula1>
-          <xm:sqref>B6:B655</xm:sqref>
+          <xm:sqref>B6:B652</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -44447,7 +44255,7 @@
       </c>
       <c r="G49" s="16"/>
     </row>
-    <row r="50" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
update to xlsx files to remove headers
</commit_message>
<xml_diff>
--- a/example/Sample_Bar_template_v2023_1.xlsx
+++ b/example/Sample_Bar_template_v2023_1.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brist\Documents\GitHub\rsoxs_scans\example\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828CE2AC-039E-41D3-B242-9110BA595953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDDFF42-B9C6-45A6-8648-33330E09C3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39220" yWindow="-4520" windowWidth="30950" windowHeight="16050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39450" yWindow="-4290" windowWidth="30950" windowHeight="16050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -32,33 +27,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={AF21D3A3-C285-426E-9589-5D767983D246}</author>
-    <author>tc={58AA31AC-0C15-477E-8808-CBF39EC24C66}</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AF21D3A3-C285-426E-9589-5D767983D246}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    The Jupyterhub tester should read cell B4 first and compare against a list of valid sheets that is updated with each new version of the spreadsheet that is released.</t>
-      </text>
-    </comment>
-    <comment ref="F17" authorId="1" shapeId="0" xr:uid="{58AA31AC-0C15-477E-8808-CBF39EC24C66}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Clarify 0 vs 180 etc.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1139,9 +1107,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Patel, Bijal B. (Fed)" id="{279F44F1-578F-4938-9B3C-F47DAE1EE193}" userId="Patel, Bijal B. (Fed)" providerId="None"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1439,17 +1405,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" dT="2023-01-04T20:16:19.03" personId="{279F44F1-578F-4938-9B3C-F47DAE1EE193}" id="{AF21D3A3-C285-426E-9589-5D767983D246}">
-    <text>The Jupyterhub tester should read cell B4 first and compare against a list of valid sheets that is updated with each new version of the spreadsheet that is released.</text>
-  </threadedComment>
-  <threadedComment ref="F17" dT="2023-01-04T20:35:24.66" personId="{279F44F1-578F-4938-9B3C-F47DAE1EE193}" id="{58AA31AC-0C15-477E-8808-CBF39EC24C66}">
-    <text>Clarify 0 vs 180 etc.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
@@ -42847,7 +42802,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B514C0-9C99-41C6-BC0F-B41277EB212E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B514C0-9C99-41C6-BC0F-B41277EB212E}">
   <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -44422,6 +44377,5 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>